<commit_message>
Updated VRE capacity in nordics.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-vre.xlsx
+++ b/input/capacity/additional-units-vre.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Remove_units_by_node" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$35</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$39</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="32">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -261,13 +261,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -311,7 +311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -333,7 +333,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -355,7 +355,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -376,7 +376,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -397,7 +397,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -420,7 +420,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -443,7 +443,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -464,7 +464,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -485,7 +485,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -502,7 +502,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -519,7 +519,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -536,7 +536,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
@@ -553,7 +553,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -571,7 +571,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -589,7 +589,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -607,7 +607,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -625,7 +625,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
@@ -642,7 +642,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -659,7 +659,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
@@ -676,7 +676,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
@@ -707,7 +707,7 @@
         <v>2040</v>
       </c>
       <c r="F22" s="1" t="n">
-        <v>3000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,7 +761,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -778,7 +778,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -795,7 +795,7 @@
         <v>29000</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -812,7 +812,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -829,7 +829,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -932,64 +932,191 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="A36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>5800</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="A37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>13100</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="1"/>
+      <c r="A38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>7200</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="1"/>
+      <c r="A39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>3900</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="1"/>
+      <c r="A40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>11000</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="A41" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>3000</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+      <c r="A42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>8000</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="1"/>
+      <c r="A43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>4000</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
+      <c r="A45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>3000</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="A46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>8000</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1"/>
@@ -1110,7 +1237,13 @@
       <c r="F66" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J35"/>
+  <autoFilter ref="A1:J39">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="2040"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
updated wind PL, BE
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-vre.xlsx
+++ b/input/capacity/additional-units-vre.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Capacity" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$48</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$56</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="35">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -119,6 +119,15 @@
   </si>
   <si>
     <t xml:space="preserve">UK00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NON1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE00</t>
   </si>
 </sst>
 </file>
@@ -266,7 +275,7 @@
   <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
+      <selection pane="topLeft" activeCell="D58" activeCellId="0" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -588,7 +597,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -606,7 +615,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -709,7 +718,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
@@ -828,7 +837,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -845,7 +854,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
@@ -862,7 +871,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>18</v>
       </c>
@@ -896,7 +905,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
@@ -913,7 +922,7 @@
         <v>6200</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
@@ -930,7 +939,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
@@ -947,7 +956,7 @@
         <v>7600</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>18</v>
       </c>
@@ -1032,7 +1041,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>16</v>
       </c>
@@ -1049,7 +1058,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>18</v>
       </c>
@@ -1080,7 +1089,7 @@
         <v>2040</v>
       </c>
       <c r="F44" s="1" t="n">
-        <v>8000</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,49 +1160,127 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="1"/>
+    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>4770</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>15000</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="1"/>
+      <c r="A55" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <v>6500</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1"/>
-      <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="1"/>
     </row>
@@ -1247,18 +1334,10 @@
       <c r="F64" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J48">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="2040"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:J56">
     <filterColumn colId="0">
       <filters>
-        <filter val="SE01"/>
-        <filter val="SE02"/>
-        <filter val="SE03"/>
-        <filter val="SE04"/>
+        <filter val="PL00"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Small adjustments to solar PV DK.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-vre.xlsx
+++ b/input/capacity/additional-units-vre.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="35">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -378,10 +378,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B104" activeCellId="0" sqref="B104"/>
+      <selection pane="topLeft" activeCell="D96" activeCellId="0" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1079,7 +1079,7 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -1093,10 +1093,10 @@
         <v>2040</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>20</v>
       </c>
@@ -1110,10 +1110,10 @@
         <v>2040</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -1127,10 +1127,10 @@
         <v>2040</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7300</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>20</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>2040</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>2000</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1480,7 +1480,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
         <v>14</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>14</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>15</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>15</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>16</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>5300</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>16</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>16</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>18</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>18</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>18</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
         <v>20</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
         <v>20</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
         <v>20</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
         <v>19</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
         <v>19</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
         <v>19</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>21</v>
       </c>
@@ -1973,20 +1973,52 @@
         <v>22000</v>
       </c>
     </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E91" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E92" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <v>5600</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J90">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="DKE1"/>
+        <filter val="DKW1"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4">
       <filters blank="1">
         <filter val="2030"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="0">
-      <filters>
-        <filter val="PL00"/>
-        <filter val="SE01"/>
-        <filter val="SE02"/>
-        <filter val="SE03"/>
-        <filter val="SE04"/>
+        <filter val="2040"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Increased offshore wind DE, UK, PL.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-vre.xlsx
+++ b/input/capacity/additional-units-vre.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Capacity" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$91</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$97</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="35">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -378,10 +378,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A93" activeCellId="0" sqref="A93"/>
+      <selection pane="topLeft" activeCell="H97" activeCellId="0" sqref="H97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -425,7 +425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -447,7 +447,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -807,7 +807,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -892,7 +892,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -909,7 +909,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -926,7 +926,7 @@
         <v>15300</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -994,7 +994,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>31</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>10</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
         <v>10</v>
       </c>
@@ -2014,16 +2014,140 @@
       <c r="E92" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="F92" s="0" t="n">
+      <c r="F92" s="1" t="n">
         <v>24000</v>
       </c>
     </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E93" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F93" s="1" t="n">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E94" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F94" s="1" t="n">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E95" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F95" s="1" t="n">
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E96" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F96" s="1" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F97" s="1" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F98" s="1" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E99" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F99" s="1" t="n">
+        <v>7000</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J91">
+  <autoFilter ref="A1:J97">
     <filterColumn colId="0">
       <filters>
-        <filter val="FI00"/>
+        <filter val="DE00"/>
         <filter val="UK00"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Offshore Wind"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Increased offshore wind NL.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-vre.xlsx
+++ b/input/capacity/additional-units-vre.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Capacity" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$97</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$99</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="35">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -378,10 +378,10 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J99"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H97" activeCellId="0" sqref="H97"/>
+      <selection pane="topLeft" activeCell="H98" activeCellId="0" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+      <c r="A94" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C94" s="1" t="s">
@@ -2053,7 +2053,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+      <c r="A95" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C95" s="1" t="s">
@@ -2070,7 +2070,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+      <c r="A96" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C96" s="1" t="s">
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+      <c r="A97" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C97" s="1" t="s">
@@ -2104,7 +2104,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+      <c r="A98" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C98" s="1" t="s">
@@ -2121,7 +2121,7 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+      <c r="A99" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C99" s="1" t="s">
@@ -2137,8 +2137,42 @@
         <v>7000</v>
       </c>
     </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E100" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F100" s="1" t="n">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E101" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F101" s="1" t="n">
+        <v>20000</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J97">
+  <autoFilter ref="A1:J99">
     <filterColumn colId="0">
       <filters>
         <filter val="DE00"/>

</xml_diff>

<commit_message>
Added some PV capacity in DE00.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-vre.xlsx
+++ b/input/capacity/additional-units-vre.xlsx
@@ -381,7 +381,7 @@
   <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C114" activeCellId="0" sqref="C114"/>
+      <selection pane="topLeft" activeCell="G105" activeCellId="0" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -633,7 +633,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -650,7 +650,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -875,7 +875,7 @@
         <v>29000</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -889,7 +889,7 @@
         <v>2025</v>
       </c>
       <c r="F26" s="1" t="n">
-        <v>80000</v>
+        <v>89000</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,7 +1797,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
         <v>20</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
         <v>19</v>
       </c>
@@ -2207,12 +2207,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J103">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="DKE1"/>
-        <filter val="DKW1"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="2">
       <filters>
         <filter val="Solar PV"/>
@@ -2220,7 +2214,14 @@
     </filterColumn>
     <filterColumn colId="4">
       <filters>
-        <filter val="2030"/>
+        <filter val="2025"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="0">
+      <filters>
+        <filter val="DE00"/>
+        <filter val="DKE1"/>
+        <filter val="DKW1"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Correcting error in additional-units-vre.xlsx.
</commit_message>
<xml_diff>
--- a/input/capacity/additional-units-vre.xlsx
+++ b/input/capacity/additional-units-vre.xlsx
@@ -10,9 +10,6 @@
   <sheets>
     <sheet name="Capacity" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Capacity!$A$1:$J$111</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -263,10 +260,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
@@ -375,13 +368,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H107" activeCellId="0" sqref="H107"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -425,7 +418,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -447,7 +440,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -469,7 +462,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -490,7 +483,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -511,7 +504,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -534,7 +527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -557,7 +550,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -578,7 +571,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -599,7 +592,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -616,7 +609,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -633,7 +626,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -650,7 +643,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -667,7 +660,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -685,7 +678,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -703,7 +696,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -721,7 +714,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -739,7 +732,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -756,7 +749,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -773,7 +766,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -790,7 +783,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -807,7 +800,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -824,7 +817,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
@@ -841,7 +834,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -858,7 +851,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -875,7 +868,7 @@
         <v>29000</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -892,7 +885,7 @@
         <v>89000</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -909,7 +902,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -994,7 +987,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
@@ -1011,7 +1004,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
@@ -1028,7 +1021,7 @@
         <v>5980</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
@@ -1045,7 +1038,7 @@
         <v>13600</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
@@ -1062,7 +1055,7 @@
         <v>7400</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>18</v>
       </c>
@@ -1079,7 +1072,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -1096,7 +1089,7 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>20</v>
       </c>
@@ -1113,7 +1106,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -1130,7 +1123,7 @@
         <v>7300</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>20</v>
       </c>
@@ -1147,7 +1140,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>16</v>
       </c>
@@ -1164,7 +1157,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>18</v>
       </c>
@@ -1181,7 +1174,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>28</v>
       </c>
@@ -1198,7 +1191,7 @@
         <v>6200</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>22</v>
       </c>
@@ -1215,7 +1208,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
@@ -1232,7 +1225,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
@@ -1249,7 +1242,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>32</v>
       </c>
@@ -1266,7 +1259,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>33</v>
       </c>
@@ -1283,7 +1276,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>28</v>
       </c>
@@ -1300,7 +1293,7 @@
         <v>4770</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>32</v>
       </c>
@@ -1317,7 +1310,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>33</v>
       </c>
@@ -1334,60 +1327,82 @@
         <v>900</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="1"/>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>22000</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="s">
-        <v>25</v>
+      <c r="A55" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>48000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F56" s="1" t="n">
-        <v>22000</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+        <v>2030</v>
+      </c>
+      <c r="F56" s="2" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>26</v>
+      <c r="C57" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>27</v>
@@ -1395,15 +1410,17 @@
       <c r="E57" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="F57" s="1" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="F57" s="2" t="n">
+        <v>11000</v>
+      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -1412,15 +1429,13 @@
       <c r="E58" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="F58" s="2" t="n">
-        <v>4000</v>
-      </c>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="s">
-        <v>10</v>
+      <c r="F58" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>11</v>
@@ -1431,17 +1446,15 @@
       <c r="E59" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="F59" s="2" t="n">
-        <v>11000</v>
-      </c>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="F59" s="1" t="n">
+        <v>3850</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -1451,12 +1464,12 @@
         <v>2030</v>
       </c>
       <c r="F60" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>11</v>
@@ -1464,19 +1477,19 @@
       <c r="D61" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E61" s="2" t="n">
+      <c r="E61" s="1" t="n">
         <v>2030</v>
       </c>
       <c r="F61" s="1" t="n">
-        <v>3850</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8700</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>27</v>
@@ -1485,32 +1498,32 @@
         <v>2030</v>
       </c>
       <c r="F62" s="1" t="n">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E63" s="1" t="n">
+      <c r="E63" s="2" t="n">
         <v>2030</v>
       </c>
       <c r="F63" s="1" t="n">
-        <v>8700</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>11</v>
+      <c r="C64" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>27</v>
@@ -1519,66 +1532,66 @@
         <v>2030</v>
       </c>
       <c r="F64" s="1" t="n">
-        <v>4800</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E65" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="1" t="n">
         <v>2030</v>
       </c>
       <c r="F65" s="1" t="n">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E66" s="2" t="n">
+      <c r="E66" s="1" t="n">
         <v>2030</v>
       </c>
       <c r="F66" s="1" t="n">
-        <v>3900</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D67" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E67" s="1" t="n">
         <v>2030</v>
       </c>
       <c r="F67" s="1" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>27</v>
@@ -1587,15 +1600,15 @@
         <v>2030</v>
       </c>
       <c r="F68" s="1" t="n">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>27</v>
@@ -1604,15 +1617,15 @@
         <v>2030</v>
       </c>
       <c r="F69" s="1" t="n">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>13</v>
+      <c r="C70" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>27</v>
@@ -1621,15 +1634,15 @@
         <v>2030</v>
       </c>
       <c r="F70" s="1" t="n">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>27</v>
@@ -1638,15 +1651,15 @@
         <v>2030</v>
       </c>
       <c r="F71" s="1" t="n">
-        <v>3700</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>27</v>
@@ -1655,15 +1668,15 @@
         <v>2030</v>
       </c>
       <c r="F72" s="1" t="n">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>13</v>
+      <c r="C73" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>27</v>
@@ -1672,32 +1685,32 @@
         <v>2030</v>
       </c>
       <c r="F73" s="1" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E74" s="1" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F74" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E74" s="1" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F74" s="1" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>27</v>
@@ -1706,15 +1719,15 @@
         <v>2030</v>
       </c>
       <c r="F75" s="1" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>13</v>
+      <c r="C76" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>27</v>
@@ -1723,15 +1736,15 @@
         <v>2030</v>
       </c>
       <c r="F76" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
-        <v>32</v>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>27</v>
@@ -1740,15 +1753,15 @@
         <v>2030</v>
       </c>
       <c r="F77" s="1" t="n">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>26</v>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>27</v>
@@ -1757,15 +1770,15 @@
         <v>2030</v>
       </c>
       <c r="F78" s="1" t="n">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>13</v>
+      <c r="C79" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>27</v>
@@ -1774,15 +1787,15 @@
         <v>2030</v>
       </c>
       <c r="F79" s="1" t="n">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>27</v>
@@ -1791,15 +1804,15 @@
         <v>2030</v>
       </c>
       <c r="F80" s="1" t="n">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>27</v>
@@ -1808,15 +1821,15 @@
         <v>2030</v>
       </c>
       <c r="F81" s="1" t="n">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>13</v>
+      <c r="C82" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>27</v>
@@ -1825,15 +1838,15 @@
         <v>2030</v>
       </c>
       <c r="F82" s="1" t="n">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="s">
-        <v>19</v>
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>27</v>
@@ -1842,15 +1855,15 @@
         <v>2030</v>
       </c>
       <c r="F83" s="1" t="n">
-        <v>10200</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>27</v>
@@ -1859,12 +1872,12 @@
         <v>2030</v>
       </c>
       <c r="F84" s="1" t="n">
-        <v>4300</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>13</v>
@@ -1879,9 +1892,9 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2" t="s">
-        <v>24</v>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>13</v>
@@ -1893,12 +1906,12 @@
         <v>2030</v>
       </c>
       <c r="F86" s="1" t="n">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
-        <v>23</v>
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>13</v>
@@ -1906,305 +1919,305 @@
       <c r="D87" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E87" s="1" t="n">
-        <v>2030</v>
+      <c r="E87" s="2" t="n">
+        <v>2040</v>
       </c>
       <c r="F87" s="1" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E88" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F88" s="1" t="n">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E89" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F89" s="1" t="n">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F90" s="1" t="n">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E91" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F91" s="1" t="n">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E92" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F92" s="1" t="n">
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E93" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F93" s="1" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E94" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F94" s="1" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E88" s="1" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F88" s="1" t="n">
-        <v>36000</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E89" s="2" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F89" s="1" t="n">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E90" s="2" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F90" s="1" t="n">
-        <v>6300</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E91" s="2" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F91" s="1" t="n">
-        <v>24000</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E92" s="2" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F92" s="1" t="n">
+      <c r="C95" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E95" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F95" s="1" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E96" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F96" s="1" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F97" s="1" t="n">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F98" s="1" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E99" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F99" s="1" t="n">
+        <v>85000</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E100" s="2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="F100" s="1" t="n">
         <v>35000</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E93" s="2" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F93" s="1" t="n">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E94" s="2" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F94" s="1" t="n">
-        <v>28000</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E95" s="2" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F95" s="1" t="n">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E96" s="2" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F96" s="1" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E97" s="2" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F97" s="1" t="n">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E98" s="2" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F98" s="1" t="n">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E99" s="2" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F99" s="1" t="n">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E100" s="2" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F100" s="1" t="n">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D101" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E101" s="2" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="F101" s="1" t="n">
-        <v>85000</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E102" s="2" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="F102" s="1" t="n">
-        <v>35000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D103" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D103" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E103" s="2" t="n">
         <v>2040</v>
       </c>
       <c r="F103" s="1" t="n">
-        <v>4000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D104" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E104" s="2" t="n">
         <v>2040</v>
       </c>
       <c r="F104" s="1" t="n">
-        <v>500</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>13</v>
@@ -2216,29 +2229,29 @@
         <v>2040</v>
       </c>
       <c r="F105" s="1" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E106" s="2" t="n">
-        <v>2040</v>
+        <v>30</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E106" s="1" t="n">
+        <v>2030</v>
       </c>
       <c r="F106" s="1" t="n">
-        <v>1800</v>
+        <v>147000</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>13</v>
@@ -2246,94 +2259,48 @@
       <c r="D107" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E107" s="2" t="n">
-        <v>2040</v>
+      <c r="E107" s="1" t="n">
+        <v>2030</v>
       </c>
       <c r="F107" s="1" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E108" s="2" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F108" s="1" t="n">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C108" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E108" s="1" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F108" s="1" t="n">
-        <v>147000</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C109" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E109" s="1" t="n">
-        <v>2030</v>
+      <c r="E109" s="2" t="n">
+        <v>2040</v>
       </c>
       <c r="F109" s="1" t="n">
-        <v>33000</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E110" s="2" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F110" s="1" t="n">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E111" s="2" t="n">
-        <v>2040</v>
-      </c>
-      <c r="F111" s="1" t="n">
-        <v>190000</v>
+        <v>180000</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J111">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="2040"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Solar PV"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2341,6 +2308,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>